<commit_message>
Demo with incrementing PC
Very slow clock so we can watch the PC but still does not perform instructions
</commit_message>
<xml_diff>
--- a/Demo Planning/EC551_Lab1_TestProgram_Sequence.xlsx
+++ b/Demo Planning/EC551_Lab1_TestProgram_Sequence.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad\eng\users\c\n\cnaught1\My Documents\GitHub\EC551_Labs\Demo Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\EC551\Labs\Lab1\Final Copy\EC551_Labs\Demo Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476CE0D6-27BB-48A4-9C7D-D073ED7CC0B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4795F793-EC8F-4115-9A5C-5D4CAD6E9688}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -960,14 +960,15 @@
   </sheetPr>
   <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" style="4" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="4" customWidth="1"/>

</xml_diff>